<commit_message>
Clean code for the marginal values
</commit_message>
<xml_diff>
--- a/models/tests/results_bounds.xlsx
+++ b/models/tests/results_bounds.xlsx
@@ -527,13 +527,13 @@
         <v>-441003.5953130126</v>
       </c>
       <c r="C5" t="n">
-        <v>5516996.404686987</v>
+        <v>-441003.5953130126</v>
       </c>
       <c r="D5" t="n">
-        <v>5516996.404686987</v>
+        <v>-441003.5953130126</v>
       </c>
       <c r="E5" t="n">
-        <v>5516996.404686987</v>
+        <v>-441003.5953130126</v>
       </c>
     </row>
     <row r="6">
@@ -755,13 +755,13 @@
         <v>-4134175.702280757</v>
       </c>
       <c r="C17" t="n">
-        <v>-3384599.702280757</v>
+        <v>-4134175.702280757</v>
       </c>
       <c r="D17" t="n">
-        <v>-3384599.702280757</v>
+        <v>-4134175.702280757</v>
       </c>
       <c r="E17" t="n">
-        <v>-3384599.702280753</v>
+        <v>-4134175.702280753</v>
       </c>
     </row>
     <row r="18">
@@ -853,7 +853,7 @@
         <v>287.1054198927933</v>
       </c>
       <c r="D22" t="n">
-        <v>3957.979999999997</v>
+        <v>287.1054198927933</v>
       </c>
       <c r="E22" t="n">
         <v>287.1054198927933</v>
@@ -1192,13 +1192,13 @@
         <v>-294070</v>
       </c>
       <c r="C40" t="n">
-        <v>-294060</v>
+        <v>-294070</v>
       </c>
       <c r="D40" t="n">
-        <v>-2899.252787650353</v>
+        <v>-294070</v>
       </c>
       <c r="E40" t="n">
-        <v>-294059.9999999999</v>
+        <v>-294069.9999999999</v>
       </c>
     </row>
     <row r="41">
@@ -1461,7 +1461,7 @@
         <v>-8471.957300266935</v>
       </c>
       <c r="D54" t="n">
-        <v>-8471.957300266935</v>
+        <v>-8471.957300271906</v>
       </c>
       <c r="E54" t="n">
         <v>-8471.957300271079</v>

</xml_diff>